<commit_message>
added main file to take in input values and add in defaults where necessary
</commit_message>
<xml_diff>
--- a/BigFan/inputs.xlsx
+++ b/BigFan/inputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>rr</t>
   </si>
@@ -81,9 +81,6 @@
     <t>off</t>
   </si>
   <si>
-    <t>Random Start</t>
-  </si>
-  <si>
     <t>axial induction factor</t>
   </si>
   <si>
@@ -319,6 +316,18 @@
   </si>
   <si>
     <t>mlDenom</t>
+  </si>
+  <si>
+    <t>Description of Variable Name</t>
+  </si>
+  <si>
+    <t>RandomStart</t>
+  </si>
+  <si>
+    <t>Variable Name in Code</t>
+  </si>
+  <si>
+    <t>User input values</t>
   </si>
 </sst>
 </file>
@@ -658,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,195 +680,195 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>400</v>
+      </c>
+      <c r="F3">
+        <v>600</v>
+      </c>
+      <c r="G3">
+        <v>800</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>1200</v>
+      </c>
+      <c r="J3">
+        <v>1400</v>
+      </c>
+      <c r="K3">
+        <v>1600</v>
+      </c>
+      <c r="L3">
+        <v>1800</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>40</v>
-      </c>
-      <c r="F4">
-        <v>40</v>
-      </c>
-      <c r="G4">
-        <v>40</v>
-      </c>
-      <c r="H4">
-        <v>40</v>
-      </c>
-      <c r="I4">
-        <v>40</v>
-      </c>
-      <c r="J4">
-        <v>40</v>
-      </c>
-      <c r="K4">
-        <v>40</v>
-      </c>
-      <c r="L4">
-        <v>40</v>
+        <v>101</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="I5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="K5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="L5">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0.314</v>
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="F6">
+        <v>80</v>
+      </c>
+      <c r="G6">
+        <v>80</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>80</v>
+      </c>
+      <c r="K6">
+        <v>80</v>
+      </c>
+      <c r="L6">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>2000</v>
+        <v>0.314</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>2000</v>
@@ -867,46 +876,46 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>3.5</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -914,252 +923,252 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>200</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>32</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>200</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26">
-        <v>1.2250000000000001</v>
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="b">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="C27">
+        <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28">
-        <v>17.190000000000001</v>
+        <v>53</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" t="b">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="C29">
+        <v>17.190000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>59</v>
+        <v>67</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C34">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35">
-        <v>400</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,18 +1176,18 @@
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>400</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -1186,54 +1195,54 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C40">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42">
         <v>100</v>
@@ -1244,18 +1253,18 @@
         <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C43">
-        <v>1E-3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C44">
         <v>1E-3</v>
@@ -1263,45 +1272,56 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45">
-        <v>100</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C46">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47">
-        <v>0.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
         <v>99</v>
       </c>
-      <c r="B48" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48">
+      <c r="C49">
         <v>2</v>
       </c>
     </row>

</xml_diff>